<commit_message>
planninglab highlight + affichage selection
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/FT Str.xlsx
+++ b/lib/PHPExcel/templates/FT Str.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="9645" windowHeight="11955"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="9645" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FTLCFDEF" sheetId="2" r:id="rId1"/>
+    <sheet name="FT" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">FT!$A$1:$P$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">FTLCFDEF!$A$1:$K$70</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="199">
   <si>
     <t>DONNEES EPROUVETTE</t>
   </si>
@@ -396,6 +398,444 @@
   <si>
     <t>Grey cell: unused equipement or information, unless specified -- Instructions on GPM need to be checked if checker is empty</t>
   </si>
+  <si>
+    <t>Grey cell : unused equipement or information (unless specified) -- Instructions on GPM need to be checked if checker is empty</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Estimated</t>
+  </si>
+  <si>
+    <t>Checker</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>Fracture</t>
+  </si>
+  <si>
+    <r>
+      <t>Rupture-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ERT(kN)</t>
+    </r>
+  </si>
+  <si>
+    <t>Duration (h)</t>
+  </si>
+  <si>
+    <t>Final Cycle</t>
+  </si>
+  <si>
+    <t>MINIMUM</t>
+  </si>
+  <si>
+    <t>End of test</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>STRAP</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>After STL</t>
+  </si>
+  <si>
+    <t>Before STL</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Corrected</t>
+  </si>
+  <si>
+    <t>Cust</t>
+  </si>
+  <si>
+    <t>Temperature (°C)</t>
+  </si>
+  <si>
+    <t>STL REALISE</t>
+  </si>
+  <si>
+    <t>Fréquency (Hz)</t>
+  </si>
+  <si>
+    <t>STL requirement</t>
+  </si>
+  <si>
+    <t>Switch to Load</t>
+  </si>
+  <si>
+    <t>(%)</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Check</t>
+    </r>
+  </si>
+  <si>
+    <t>T° Alarm</t>
+  </si>
+  <si>
+    <t>(kN)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Min (%)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Max (%)</t>
+    </r>
+  </si>
+  <si>
+    <t>(mm)</t>
+  </si>
+  <si>
+    <t>Disp</t>
+  </si>
+  <si>
+    <t>UnderPeak</t>
+  </si>
+  <si>
+    <t>Cycle Counting</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>st</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> cycle</t>
+    </r>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Specimen Temperature</t>
+  </si>
+  <si>
+    <t>Dilatation</t>
+  </si>
+  <si>
+    <t>Stabilisation Time</t>
+  </si>
+  <si>
+    <t>Controle Temperature</t>
+  </si>
+  <si>
+    <t>Nb strap</t>
+  </si>
+  <si>
+    <t>Controle</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>Ramp to Temp</t>
+  </si>
+  <si>
+    <r>
+      <t>Modulus</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="7"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ET</t>
+    </r>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <r>
+      <t>Modulus</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="7"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>RT</t>
+    </r>
+  </si>
+  <si>
+    <t>Lo</t>
+  </si>
+  <si>
+    <t>End level (%)</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Runout</t>
+  </si>
+  <si>
+    <t>Dimension 3</t>
+  </si>
+  <si>
+    <t>Dimension 2</t>
+  </si>
+  <si>
+    <t>Dimension 1</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Dimensionnal (mm)</t>
+  </si>
+  <si>
+    <t>Test Informations</t>
+  </si>
+  <si>
+    <t>Str</t>
+  </si>
+  <si>
+    <t>Loa</t>
+  </si>
+  <si>
+    <t>Temp Acq</t>
+  </si>
+  <si>
+    <t>Oscilloscope</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Sens.</t>
+  </si>
+  <si>
+    <t>Conv.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>Cooling</t>
+  </si>
+  <si>
+    <t>Heating</t>
+  </si>
+  <si>
+    <t>Tool Bot</t>
+  </si>
+  <si>
+    <t>Tool Top</t>
+  </si>
+  <si>
+    <t>Frame Informations</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(YYYY-MM-DD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Specimen) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Checker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF8497B0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Test)</t>
+    </r>
+  </si>
+  <si>
+    <t>Raw Data</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Test Number</t>
+  </si>
+  <si>
+    <t>File Number</t>
+  </si>
+  <si>
+    <t>Specimen</t>
+  </si>
+  <si>
+    <t>Prefixe</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>FT - 48558</t>
+  </si>
+  <si>
+    <t>Strain Control Fatigue Test</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +847,7 @@
     <numFmt numFmtId="166" formatCode="###\ ###\ ###\ ###\ ###\ "/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="41">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -478,8 +918,182 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="MS Sans Serif"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF8E98A5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF223962"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8E98A5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF203764"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8497B0"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="7"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8E98A5"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF8497B0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF44546A"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,8 +1106,14 @@
         <bgColor indexed="22"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8497B0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -942,12 +1562,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1248,6 +1998,192 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="22" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="47" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="49" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="50" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="48" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,11 +2209,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1591,6 +2542,95 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="742950" cy="762000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C884E5C4-2D54-4491-95FB-AAD76271600E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="161925"/>
+          <a:ext cx="742950" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66062</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="381811" cy="1938130"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{054D0D76-0B80-4B07-8689-FAED860FAF6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10924562" y="0"/>
+          <a:ext cx="381811" cy="1938130"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1947,9 +2987,11 @@
   </sheetPr>
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="96" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Z34" sqref="Z34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="10" style="10" customWidth="1"/>
@@ -1964,32 +3006,32 @@
     <col min="12" max="16384" width="8.7109375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="G2" s="75" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="132" t="s">
+    <row r="4" spans="1:14" ht="13.5" thickBot="1"/>
+    <row r="5" spans="1:14" ht="13.5" thickBot="1">
+      <c r="A5" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="134"/>
-      <c r="H5" s="132" t="s">
+      <c r="B5" s="207"/>
+      <c r="C5" s="207"/>
+      <c r="D5" s="207"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="208"/>
+      <c r="H5" s="206" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
-      <c r="K5" s="134"/>
-    </row>
-    <row r="6" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="207"/>
+      <c r="J5" s="207"/>
+      <c r="K5" s="208"/>
+    </row>
+    <row r="6" spans="1:14" ht="6.75" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -2001,7 +3043,7 @@
       <c r="J6" s="20"/>
       <c r="K6" s="23"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="14" t="s">
         <v>19</v>
       </c>
@@ -2017,7 +3059,7 @@
       <c r="J7" s="62"/>
       <c r="K7" s="63"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="14" t="s">
         <v>20</v>
       </c>
@@ -2033,7 +3075,7 @@
       <c r="J8" s="64"/>
       <c r="K8" s="65"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
@@ -2049,7 +3091,7 @@
       <c r="J9" s="64"/>
       <c r="K9" s="65"/>
     </row>
-    <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="13.5" thickBot="1">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2065,7 +3107,7 @@
       </c>
       <c r="K10" s="65"/>
     </row>
-    <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="13.5" thickBot="1">
       <c r="H11" s="14" t="s">
         <v>7</v>
       </c>
@@ -2073,14 +3115,14 @@
       <c r="J11" s="62"/>
       <c r="K11" s="63"/>
     </row>
-    <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132" t="s">
+    <row r="12" spans="1:14" ht="13.5" thickBot="1">
+      <c r="A12" s="206" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="133"/>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
+      <c r="B12" s="207"/>
+      <c r="C12" s="207"/>
+      <c r="D12" s="207"/>
+      <c r="E12" s="207"/>
       <c r="F12" s="9"/>
       <c r="H12" s="14" t="s">
         <v>8</v>
@@ -2089,7 +3131,7 @@
       <c r="J12" s="64"/>
       <c r="K12" s="65"/>
     </row>
-    <row r="13" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="13.5" thickBot="1">
       <c r="A13" s="53"/>
       <c r="B13" s="54"/>
       <c r="C13" s="54"/>
@@ -2101,7 +3143,7 @@
       <c r="J13" s="80"/>
       <c r="K13" s="81"/>
     </row>
-    <row r="14" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="13.5" thickBot="1">
       <c r="A14" s="14" t="s">
         <v>11</v>
       </c>
@@ -2120,7 +3162,7 @@
       <c r="K14" s="48"/>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="13.5" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
@@ -2131,15 +3173,15 @@
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="63"/>
-      <c r="H15" s="132" t="s">
+      <c r="H15" s="206" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
-      <c r="K15" s="134"/>
+      <c r="I15" s="207"/>
+      <c r="J15" s="207"/>
+      <c r="K15" s="208"/>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="14" t="s">
         <v>24</v>
       </c>
@@ -2160,7 +3202,7 @@
       <c r="K16" s="63"/>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="14" t="s">
         <v>25</v>
       </c>
@@ -2178,7 +3220,7 @@
       <c r="J17" s="64"/>
       <c r="K17" s="65"/>
     </row>
-    <row r="18" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="14.25" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="82"/>
       <c r="C18" s="15"/>
@@ -2194,7 +3236,7 @@
       </c>
       <c r="K18" s="63"/>
     </row>
-    <row r="19" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="3.75" customHeight="1" thickBot="1">
       <c r="A19" s="35"/>
       <c r="B19" s="83"/>
       <c r="C19" s="83"/>
@@ -2206,7 +3248,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="16"/>
     </row>
-    <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="13.5" thickBot="1">
       <c r="A20" s="37"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2220,15 +3262,15 @@
       </c>
       <c r="K20" s="84"/>
     </row>
-    <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="132" t="s">
+    <row r="21" spans="1:13" ht="13.5" thickBot="1">
+      <c r="A21" s="206" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="133"/>
-      <c r="C21" s="133"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="133"/>
-      <c r="F21" s="134"/>
+      <c r="B21" s="207"/>
+      <c r="C21" s="207"/>
+      <c r="D21" s="207"/>
+      <c r="E21" s="207"/>
+      <c r="F21" s="208"/>
       <c r="H21" s="14" t="s">
         <v>12</v>
       </c>
@@ -2238,7 +3280,7 @@
       </c>
       <c r="K21" s="86"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="24"/>
       <c r="C22" s="15"/>
       <c r="D22" s="20"/>
@@ -2253,7 +3295,7 @@
       </c>
       <c r="K22" s="65"/>
     </row>
-    <row r="23" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="14.25" customHeight="1">
       <c r="A23" s="14" t="s">
         <v>98</v>
       </c>
@@ -2274,7 +3316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="13.5" customHeight="1">
       <c r="A24" s="14" t="s">
         <v>97</v>
       </c>
@@ -2293,7 +3335,7 @@
       <c r="J24" s="89"/>
       <c r="K24" s="90"/>
     </row>
-    <row r="25" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="13.5" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>99</v>
       </c>
@@ -2312,7 +3354,7 @@
       <c r="J25" s="91"/>
       <c r="K25" s="92"/>
     </row>
-    <row r="26" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="13.5" customHeight="1">
       <c r="A26" s="14"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
@@ -2324,7 +3366,7 @@
       <c r="J26" s="91"/>
       <c r="K26" s="92"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" s="2"/>
       <c r="B27" s="6" t="s">
         <v>46</v>
@@ -2342,7 +3384,7 @@
       <c r="J27" s="93"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
@@ -2363,7 +3405,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -2382,7 +3424,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
@@ -2401,7 +3443,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="2"/>
       <c r="B31" s="103"/>
       <c r="C31" s="103"/>
@@ -2415,7 +3457,7 @@
       <c r="J31" s="91"/>
       <c r="K31" s="92"/>
     </row>
-    <row r="32" spans="1:13" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="3" customHeight="1" thickBot="1">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -2427,7 +3469,7 @@
       <c r="J32" s="104"/>
       <c r="K32" s="105"/>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2440,11 +3482,11 @@
       <c r="J33" s="18"/>
       <c r="K33" s="106"/>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="137" t="s">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A34" s="211" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="138"/>
+      <c r="B34" s="212"/>
       <c r="C34" s="28"/>
       <c r="D34" s="56"/>
       <c r="E34" s="74" t="s">
@@ -2459,7 +3501,7 @@
       <c r="J34" s="68"/>
       <c r="K34" s="30"/>
     </row>
-    <row r="35" spans="1:19" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="6.75" customHeight="1">
       <c r="A35" s="29"/>
       <c r="B35" s="30"/>
       <c r="C35" s="28"/>
@@ -2472,7 +3514,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="61"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19">
       <c r="A36" s="14" t="s">
         <v>87</v>
       </c>
@@ -2493,7 +3535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19">
       <c r="A37" s="14" t="s">
         <v>88</v>
       </c>
@@ -2515,7 +3557,7 @@
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1">
       <c r="A38" s="17" t="s">
         <v>93</v>
       </c>
@@ -2535,12 +3577,12 @@
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
     </row>
-    <row r="39" spans="1:19" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="6.75" customHeight="1" thickBot="1">
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1">
       <c r="A40" s="57" t="s">
         <v>34</v>
       </c>
@@ -2558,7 +3600,7 @@
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="15.75">
       <c r="A41" s="34" t="s">
         <v>71</v>
       </c>
@@ -2586,7 +3628,7 @@
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1">
       <c r="A42" s="17" t="s">
         <v>53</v>
       </c>
@@ -2615,7 +3657,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="6" customHeight="1" thickBot="1">
       <c r="N43" s="41"/>
       <c r="O43" s="37"/>
       <c r="P43" s="37"/>
@@ -2623,7 +3665,7 @@
       <c r="R43" s="37"/>
       <c r="S43" s="15"/>
     </row>
-    <row r="44" spans="1:19" s="36" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="36" customFormat="1" ht="13.5" thickBot="1">
       <c r="A44" s="111" t="s">
         <v>73</v>
       </c>
@@ -2644,7 +3686,7 @@
       <c r="R44" s="37"/>
       <c r="S44" s="37"/>
     </row>
-    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" s="36" customFormat="1">
       <c r="A45" s="2" t="s">
         <v>74</v>
       </c>
@@ -2669,7 +3711,7 @@
       <c r="R45" s="37"/>
       <c r="S45" s="37"/>
     </row>
-    <row r="46" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" s="36" customFormat="1">
       <c r="A46" s="2" t="s">
         <v>75</v>
       </c>
@@ -2698,7 +3740,7 @@
       <c r="R46" s="37"/>
       <c r="S46" s="37"/>
     </row>
-    <row r="47" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" s="36" customFormat="1">
       <c r="A47" s="118"/>
       <c r="B47" s="117"/>
       <c r="C47" s="117"/>
@@ -2713,7 +3755,7 @@
       <c r="J47" s="121"/>
       <c r="K47" s="32"/>
     </row>
-    <row r="48" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" s="36" customFormat="1">
       <c r="A48" s="122"/>
       <c r="B48" s="123" t="s">
         <v>78</v>
@@ -2734,7 +3776,7 @@
       <c r="J48" s="64"/>
       <c r="K48" s="32"/>
     </row>
-    <row r="49" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="36" customFormat="1">
       <c r="A49" s="126" t="s">
         <v>46</v>
       </c>
@@ -2751,7 +3793,7 @@
       <c r="J49" s="64"/>
       <c r="K49" s="42"/>
     </row>
-    <row r="50" spans="1:11" s="36" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="36" customFormat="1" ht="12.75" customHeight="1">
       <c r="A50" s="130" t="s">
         <v>47</v>
       </c>
@@ -2768,7 +3810,7 @@
       <c r="J50" s="64"/>
       <c r="K50" s="42"/>
     </row>
-    <row r="51" spans="1:11" s="36" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="36" customFormat="1" ht="12.75" customHeight="1">
       <c r="A51" s="14" t="s">
         <v>51</v>
       </c>
@@ -2797,7 +3839,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="14.65" customHeight="1" thickBot="1">
       <c r="A52" s="17" t="s">
         <v>84</v>
       </c>
@@ -2826,7 +3868,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="36" customFormat="1" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="36" customFormat="1" ht="8.1" customHeight="1" thickBot="1">
       <c r="A53" s="117"/>
       <c r="B53" s="117"/>
       <c r="C53" s="117"/>
@@ -2838,7 +3880,7 @@
       <c r="I53" s="117"/>
       <c r="J53" s="117"/>
     </row>
-    <row r="54" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="13.5" thickBot="1">
       <c r="A54" s="71" t="s">
         <v>35</v>
       </c>
@@ -2850,12 +3892,12 @@
       <c r="G54" s="72"/>
       <c r="H54" s="72"/>
       <c r="I54" s="73"/>
-      <c r="J54" s="139" t="s">
+      <c r="J54" s="213" t="s">
         <v>36</v>
       </c>
-      <c r="K54" s="140"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K54" s="214"/>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="14" t="s">
         <v>39</v>
       </c>
@@ -2875,7 +3917,7 @@
       </c>
       <c r="K55" s="27"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="14"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
@@ -2890,7 +3932,7 @@
       <c r="J56" s="69"/>
       <c r="K56" s="131"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="14" t="s">
         <v>40</v>
       </c>
@@ -2909,7 +3951,7 @@
       </c>
       <c r="K57" s="16"/>
     </row>
-    <row r="58" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="6" customHeight="1">
       <c r="A58" s="14"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -2922,7 +3964,7 @@
       <c r="J58" s="26"/>
       <c r="K58" s="27"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="14" t="s">
         <v>100</v>
       </c>
@@ -2939,7 +3981,7 @@
       <c r="J59" s="69"/>
       <c r="K59" s="66"/>
     </row>
-    <row r="60" spans="1:11" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="5.25" customHeight="1" thickBot="1">
       <c r="A60" s="17"/>
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
@@ -2949,11 +3991,11 @@
       <c r="G60" s="18"/>
       <c r="H60" s="18"/>
       <c r="I60" s="18"/>
-      <c r="J60" s="135"/>
-      <c r="K60" s="136"/>
-    </row>
-    <row r="61" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J60" s="209"/>
+      <c r="K60" s="210"/>
+    </row>
+    <row r="61" spans="1:11" ht="6" customHeight="1" thickBot="1"/>
+    <row r="62" spans="1:11">
       <c r="A62" s="22" t="s">
         <v>44</v>
       </c>
@@ -2968,8 +4010,8 @@
       <c r="J62" s="25"/>
       <c r="K62" s="23"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="141"/>
+    <row r="63" spans="1:11">
+      <c r="A63" s="132"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
@@ -2981,7 +4023,7 @@
       <c r="J63" s="15"/>
       <c r="K63" s="16"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="14"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -2994,7 +4036,7 @@
       <c r="J64" s="15"/>
       <c r="K64" s="16"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12">
       <c r="A65" s="14"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
@@ -3007,7 +4049,7 @@
       <c r="J65" s="15"/>
       <c r="K65" s="16"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12">
       <c r="A66" s="14"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -3020,7 +4062,7 @@
       <c r="J66" s="15"/>
       <c r="K66" s="16"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12">
       <c r="A67" s="14"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
@@ -3033,7 +4075,7 @@
       <c r="J67" s="15"/>
       <c r="K67" s="16"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12">
       <c r="A68" s="14"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -3046,7 +4088,7 @@
       <c r="J68" s="15"/>
       <c r="K68" s="16"/>
     </row>
-    <row r="69" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="13.5" thickBot="1">
       <c r="A69" s="17"/>
       <c r="B69" s="18"/>
       <c r="C69" s="18"/>
@@ -3060,7 +4102,7 @@
       <c r="K69" s="19"/>
       <c r="L69" s="15"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12">
       <c r="A70" s="10" t="s">
         <v>107</v>
       </c>
@@ -3082,6 +4124,1118 @@
   <pageSetup paperSize="9" scale="95" orientation="portrait" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;R&amp;6 65-21-02 27_F 12 Jul 17</oddHeader>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12:P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="16" width="6.7109375" style="134" customWidth="1"/>
+    <col min="17" max="17" width="1.28515625" style="134" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" style="134"/>
+    <col min="19" max="16384" width="10.85546875" style="133"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24.75" hidden="1" customHeight="1"/>
+    <row r="2" spans="1:18" ht="60.4" customHeight="1">
+      <c r="C2" s="205" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="204"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="204"/>
+      <c r="I2" s="204"/>
+      <c r="J2" s="204"/>
+      <c r="K2" s="204"/>
+      <c r="L2" s="204"/>
+      <c r="M2" s="204"/>
+      <c r="N2" s="203"/>
+      <c r="O2" s="215" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="18" customHeight="1">
+      <c r="O3" s="215"/>
+    </row>
+    <row r="4" spans="1:18" ht="18" customHeight="1">
+      <c r="A4" s="199" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="199"/>
+      <c r="C4" s="165"/>
+      <c r="D4" s="199" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" s="146"/>
+      <c r="F4" s="165"/>
+      <c r="G4" s="199" t="s">
+        <v>194</v>
+      </c>
+      <c r="H4" s="199"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="199" t="s">
+        <v>193</v>
+      </c>
+      <c r="K4" s="199"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="199"/>
+      <c r="N4" s="201" t="s">
+        <v>192</v>
+      </c>
+      <c r="O4" s="215"/>
+    </row>
+    <row r="5" spans="1:18" ht="18.95" customHeight="1">
+      <c r="A5" s="145"/>
+      <c r="B5" s="145"/>
+      <c r="C5" s="196"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="196"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="195"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="145"/>
+      <c r="L5" s="195"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="145"/>
+      <c r="O5" s="215"/>
+    </row>
+    <row r="6" spans="1:18" ht="18.95" customHeight="1">
+      <c r="A6" s="199" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="199"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="199" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="199"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="199" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="146"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="199" t="s">
+        <v>189</v>
+      </c>
+      <c r="K6" s="146"/>
+      <c r="L6" s="198"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="197" t="s">
+        <v>188</v>
+      </c>
+      <c r="O6" s="215"/>
+    </row>
+    <row r="7" spans="1:18" ht="18.95" customHeight="1">
+      <c r="A7" s="145"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="196"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="196"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
+      <c r="L7" s="195"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="215"/>
+    </row>
+    <row r="8" spans="1:18" ht="6" customHeight="1"/>
+    <row r="9" spans="1:18" ht="15" customHeight="1">
+      <c r="A9" s="138" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="138"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="138"/>
+      <c r="O9" s="138"/>
+      <c r="P9" s="138"/>
+    </row>
+    <row r="10" spans="1:18" ht="5.25" customHeight="1"/>
+    <row r="11" spans="1:18" s="164" customFormat="1">
+      <c r="A11" s="146" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="146"/>
+      <c r="C11" s="146" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="146"/>
+      <c r="E11" s="146" t="s">
+        <v>184</v>
+      </c>
+      <c r="F11" s="146"/>
+      <c r="G11" s="146" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="146"/>
+      <c r="I11" s="194"/>
+      <c r="J11" s="161" t="s">
+        <v>182</v>
+      </c>
+      <c r="K11" s="161" t="s">
+        <v>181</v>
+      </c>
+      <c r="L11" s="161" t="s">
+        <v>180</v>
+      </c>
+      <c r="M11" s="161" t="s">
+        <v>179</v>
+      </c>
+      <c r="N11" s="161" t="s">
+        <v>178</v>
+      </c>
+      <c r="O11" s="161" t="s">
+        <v>177</v>
+      </c>
+      <c r="P11" s="160" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q11" s="136"/>
+      <c r="R11" s="136"/>
+    </row>
+    <row r="12" spans="1:18" ht="14.25">
+      <c r="A12" s="145"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="145"/>
+      <c r="I12" s="193" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="L12" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="P12" s="217" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="164" customFormat="1">
+      <c r="A13" s="146" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="146"/>
+      <c r="C13" s="146" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="146"/>
+      <c r="E13" s="146" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" s="146"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="146"/>
+      <c r="I13" s="192" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="N13" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="216" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13" s="217" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q13" s="136"/>
+      <c r="R13" s="136"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.25">
+      <c r="A14" s="145"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="145"/>
+      <c r="E14" s="145"/>
+      <c r="F14" s="145"/>
+      <c r="G14" s="145"/>
+      <c r="H14" s="145"/>
+      <c r="I14" s="191" t="s">
+        <v>171</v>
+      </c>
+      <c r="J14" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="218" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" s="219"/>
+    </row>
+    <row r="15" spans="1:18" ht="6" customHeight="1">
+      <c r="A15" s="190"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1">
+      <c r="A16" s="139" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="138"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="138"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="138"/>
+    </row>
+    <row r="17" spans="1:18" ht="5.25" customHeight="1">
+      <c r="K17" s="184"/>
+      <c r="L17" s="184"/>
+      <c r="M17" s="184"/>
+      <c r="N17" s="184"/>
+    </row>
+    <row r="18" spans="1:18" ht="12.75" customHeight="1">
+      <c r="A18" s="165"/>
+      <c r="B18" s="165"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="146" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="146" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="146"/>
+      <c r="M18" s="146"/>
+      <c r="N18" s="146"/>
+      <c r="O18" s="165"/>
+      <c r="P18" s="165"/>
+    </row>
+    <row r="19" spans="1:18" s="164" customFormat="1">
+      <c r="A19" s="146" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="146"/>
+      <c r="C19" s="146" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146" t="s">
+        <v>166</v>
+      </c>
+      <c r="F19" s="146"/>
+      <c r="G19" s="146" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="146"/>
+      <c r="I19" s="146" t="s">
+        <v>164</v>
+      </c>
+      <c r="J19" s="146"/>
+      <c r="K19" s="146" t="s">
+        <v>126</v>
+      </c>
+      <c r="L19" s="146"/>
+      <c r="M19" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="N19" s="146"/>
+      <c r="O19" s="146" t="s">
+        <v>163</v>
+      </c>
+      <c r="P19" s="146"/>
+      <c r="Q19" s="136"/>
+      <c r="R19" s="136"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="145"/>
+      <c r="B20" s="145"/>
+      <c r="C20" s="145"/>
+      <c r="D20" s="145"/>
+      <c r="E20" s="189"/>
+      <c r="F20" s="145"/>
+      <c r="G20" s="145"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="145"/>
+      <c r="L20" s="145"/>
+      <c r="M20" s="145"/>
+      <c r="N20" s="145"/>
+      <c r="O20" s="145"/>
+      <c r="P20" s="145"/>
+    </row>
+    <row r="21" spans="1:18" s="164" customFormat="1">
+      <c r="A21" s="146"/>
+      <c r="B21" s="188" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="146" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="146"/>
+      <c r="E21" s="146" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="146"/>
+      <c r="G21" s="146" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="146"/>
+      <c r="I21" s="187"/>
+      <c r="J21" s="186" t="s">
+        <v>159</v>
+      </c>
+      <c r="K21" s="146" t="s">
+        <v>46</v>
+      </c>
+      <c r="L21" s="146"/>
+      <c r="M21" s="146" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" s="146"/>
+      <c r="O21" s="146" t="s">
+        <v>158</v>
+      </c>
+      <c r="P21" s="146"/>
+      <c r="Q21" s="136"/>
+      <c r="R21" s="136"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="185" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="141" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="145"/>
+      <c r="E22" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="145"/>
+      <c r="G22" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="145"/>
+      <c r="I22" s="184" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" s="146" t="s">
+        <v>156</v>
+      </c>
+      <c r="K22" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="L22" s="145"/>
+      <c r="M22" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="N22" s="145"/>
+      <c r="O22" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="P22" s="145"/>
+    </row>
+    <row r="23" spans="1:18" ht="15.75">
+      <c r="A23" s="144" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" s="183" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="179" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="179"/>
+      <c r="E23" s="182" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" s="182"/>
+      <c r="G23" s="181"/>
+      <c r="H23" s="182"/>
+      <c r="I23" s="181"/>
+      <c r="J23" s="180" t="s">
+        <v>153</v>
+      </c>
+      <c r="K23" s="179" t="s">
+        <v>76</v>
+      </c>
+      <c r="L23" s="179"/>
+      <c r="M23" s="179" t="s">
+        <v>76</v>
+      </c>
+      <c r="N23" s="179"/>
+      <c r="O23" s="179" t="s">
+        <v>76</v>
+      </c>
+      <c r="P23" s="179"/>
+    </row>
+    <row r="24" spans="1:18" ht="5.25" customHeight="1">
+      <c r="A24" s="154"/>
+      <c r="B24" s="153"/>
+      <c r="C24" s="153"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="153"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
+      <c r="H24" s="153"/>
+      <c r="I24" s="153"/>
+      <c r="J24" s="153"/>
+      <c r="K24" s="147"/>
+      <c r="L24" s="147"/>
+      <c r="M24" s="147"/>
+      <c r="N24" s="147"/>
+      <c r="O24" s="147"/>
+      <c r="P24" s="147"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="154" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="154"/>
+      <c r="C25" s="154" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="178"/>
+      <c r="E25" s="154" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="154"/>
+      <c r="G25" s="178"/>
+      <c r="H25" s="177" t="s">
+        <v>149</v>
+      </c>
+      <c r="I25" s="177"/>
+      <c r="J25" s="146" t="s">
+        <v>148</v>
+      </c>
+      <c r="K25" s="146"/>
+      <c r="L25" s="154" t="s">
+        <v>147</v>
+      </c>
+      <c r="M25" s="154"/>
+      <c r="N25" s="154"/>
+      <c r="O25" s="154"/>
+      <c r="P25" s="154"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="154" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="148"/>
+      <c r="G26" s="148"/>
+      <c r="H26" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="148"/>
+      <c r="J26" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="K26" s="148"/>
+      <c r="L26" s="154" t="s">
+        <v>121</v>
+      </c>
+      <c r="M26" s="154"/>
+      <c r="N26" s="155" t="s">
+        <v>120</v>
+      </c>
+      <c r="O26" s="154" t="s">
+        <v>119</v>
+      </c>
+      <c r="P26" s="154"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="154" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="175"/>
+      <c r="D27" s="175"/>
+      <c r="E27" s="175"/>
+      <c r="F27" s="175"/>
+      <c r="G27" s="175"/>
+      <c r="H27" s="175"/>
+      <c r="I27" s="175"/>
+      <c r="J27" s="176"/>
+      <c r="K27" s="176"/>
+      <c r="L27" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="M27" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="N27" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="O27" s="148"/>
+      <c r="P27" s="175"/>
+    </row>
+    <row r="28" spans="1:18" ht="6" customHeight="1"/>
+    <row r="29" spans="1:18" ht="15.75">
+      <c r="A29" s="139" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="138"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="138"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
+      <c r="J29" s="138"/>
+      <c r="K29" s="138"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="138"/>
+      <c r="N29" s="138"/>
+      <c r="O29" s="138"/>
+      <c r="P29" s="138"/>
+    </row>
+    <row r="30" spans="1:18" ht="5.25" customHeight="1">
+      <c r="K30" s="165"/>
+      <c r="L30" s="165"/>
+      <c r="M30" s="165"/>
+      <c r="N30" s="165"/>
+      <c r="O30" s="165"/>
+      <c r="P30" s="165"/>
+    </row>
+    <row r="31" spans="1:18" ht="14.25">
+      <c r="A31" s="174" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="161" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="161" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="154" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="154"/>
+      <c r="H31" s="154"/>
+      <c r="I31" s="165"/>
+      <c r="K31" s="146" t="s">
+        <v>142</v>
+      </c>
+      <c r="L31" s="146"/>
+      <c r="M31" s="146" t="s">
+        <v>53</v>
+      </c>
+      <c r="N31" s="146"/>
+      <c r="O31" s="146" t="s">
+        <v>141</v>
+      </c>
+      <c r="P31" s="146"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="171" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="170" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="173" t="s">
+        <v>138</v>
+      </c>
+      <c r="G32" s="146"/>
+      <c r="H32" s="172" t="s">
+        <v>137</v>
+      </c>
+      <c r="I32" s="165"/>
+      <c r="K32" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="145"/>
+      <c r="M32" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="N32" s="145"/>
+      <c r="O32" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="P32" s="145"/>
+    </row>
+    <row r="33" spans="1:18" ht="14.25" customHeight="1">
+      <c r="A33" s="171" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="170" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="145"/>
+      <c r="G33" s="145" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33" s="146" t="s">
+        <v>135</v>
+      </c>
+      <c r="L33" s="146"/>
+      <c r="M33" s="146" t="s">
+        <v>58</v>
+      </c>
+      <c r="N33" s="146"/>
+      <c r="O33" s="146" t="s">
+        <v>134</v>
+      </c>
+      <c r="P33" s="146"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="169" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="150" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="150" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="168" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="136"/>
+      <c r="K34" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="145"/>
+      <c r="M34" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" s="145"/>
+      <c r="O34" s="167" t="s">
+        <v>50</v>
+      </c>
+      <c r="P34" s="145"/>
+    </row>
+    <row r="35" spans="1:18" ht="6" customHeight="1">
+      <c r="A35" s="136"/>
+      <c r="C35" s="136"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75">
+      <c r="A36" s="139" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="138"/>
+      <c r="C36" s="138"/>
+      <c r="D36" s="138"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="138"/>
+      <c r="H36" s="138"/>
+      <c r="I36" s="138"/>
+      <c r="J36" s="138"/>
+      <c r="K36" s="138"/>
+      <c r="L36" s="138"/>
+      <c r="M36" s="138"/>
+      <c r="N36" s="138"/>
+      <c r="O36" s="138"/>
+      <c r="P36" s="138"/>
+    </row>
+    <row r="37" spans="1:18" ht="5.25" customHeight="1"/>
+    <row r="38" spans="1:18" s="164" customFormat="1">
+      <c r="A38" s="166" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="146"/>
+      <c r="C38" s="165"/>
+      <c r="D38" s="146" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="165"/>
+      <c r="F38" s="165"/>
+      <c r="G38" s="146" t="s">
+        <v>128</v>
+      </c>
+      <c r="H38" s="165"/>
+      <c r="I38" s="146" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="146"/>
+      <c r="K38" s="165"/>
+      <c r="L38" s="146" t="s">
+        <v>127</v>
+      </c>
+      <c r="M38" s="146"/>
+      <c r="N38" s="146"/>
+      <c r="O38" s="146"/>
+      <c r="P38" s="165"/>
+      <c r="Q38" s="136"/>
+      <c r="R38" s="136"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="145"/>
+      <c r="B39" s="145"/>
+      <c r="C39" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="145"/>
+      <c r="E39" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" s="145"/>
+      <c r="H39" s="145"/>
+      <c r="I39" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="J39" s="145"/>
+      <c r="K39" s="140"/>
+      <c r="L39" s="146" t="s">
+        <v>126</v>
+      </c>
+      <c r="M39" s="146"/>
+      <c r="N39" s="146" t="s">
+        <v>125</v>
+      </c>
+      <c r="O39" s="146"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="163" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="162" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="161" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="161"/>
+      <c r="E40" s="161" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" s="160"/>
+      <c r="H40" s="146" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" s="146"/>
+      <c r="K40" s="153"/>
+      <c r="L40" s="159"/>
+      <c r="M40" s="159"/>
+      <c r="N40" s="159"/>
+      <c r="O40" s="159"/>
+      <c r="P40" s="153"/>
+    </row>
+    <row r="41" spans="1:18" ht="14.25">
+      <c r="A41" s="158" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="151"/>
+      <c r="C41" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="157"/>
+      <c r="E41" s="157" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="156"/>
+      <c r="H41" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="145"/>
+      <c r="K41" s="154" t="s">
+        <v>121</v>
+      </c>
+      <c r="L41" s="154"/>
+      <c r="M41" s="155" t="s">
+        <v>120</v>
+      </c>
+      <c r="N41" s="154" t="s">
+        <v>119</v>
+      </c>
+      <c r="O41" s="154"/>
+      <c r="P41" s="153" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="14.25">
+      <c r="A42" s="152" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="151"/>
+      <c r="C42" s="150" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="150"/>
+      <c r="E42" s="150" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="149"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="140"/>
+      <c r="K42" s="148" t="s">
+        <v>76</v>
+      </c>
+      <c r="L42" s="148"/>
+      <c r="M42" s="148"/>
+      <c r="N42" s="148"/>
+      <c r="O42" s="148"/>
+      <c r="P42" s="147"/>
+    </row>
+    <row r="43" spans="1:18" ht="6" customHeight="1"/>
+    <row r="44" spans="1:18" ht="15.75">
+      <c r="A44" s="139" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="138"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="138"/>
+      <c r="E44" s="138"/>
+      <c r="F44" s="138"/>
+      <c r="G44" s="138"/>
+      <c r="H44" s="138"/>
+      <c r="I44" s="138"/>
+      <c r="J44" s="138"/>
+      <c r="K44" s="138"/>
+      <c r="L44" s="138"/>
+      <c r="M44" s="138"/>
+      <c r="N44" s="138"/>
+      <c r="O44" s="138"/>
+      <c r="P44" s="138"/>
+    </row>
+    <row r="45" spans="1:18" ht="5.25" customHeight="1"/>
+    <row r="46" spans="1:18">
+      <c r="A46" s="146" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="146"/>
+      <c r="C46" s="146" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="146"/>
+      <c r="E46" s="146" t="s">
+        <v>115</v>
+      </c>
+      <c r="F46" s="146"/>
+      <c r="G46" s="146" t="s">
+        <v>114</v>
+      </c>
+      <c r="H46" s="146"/>
+      <c r="I46" s="146" t="s">
+        <v>113</v>
+      </c>
+      <c r="J46" s="146"/>
+      <c r="K46" s="146" t="s">
+        <v>5</v>
+      </c>
+      <c r="L46" s="146"/>
+      <c r="M46" s="146" t="s">
+        <v>112</v>
+      </c>
+      <c r="N46" s="146"/>
+      <c r="O46" s="146" t="s">
+        <v>111</v>
+      </c>
+      <c r="P46" s="146"/>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="145"/>
+      <c r="B47" s="145"/>
+      <c r="C47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="145"/>
+      <c r="E47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="F47" s="145"/>
+      <c r="G47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="145"/>
+      <c r="I47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="J47" s="145"/>
+      <c r="K47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="L47" s="145"/>
+      <c r="M47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="N47" s="145"/>
+      <c r="O47" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="P47" s="145"/>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="B48" s="144" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="141" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="141"/>
+      <c r="E48" s="141" t="s">
+        <v>76</v>
+      </c>
+      <c r="F48" s="141"/>
+      <c r="G48" s="143" t="s">
+        <v>76</v>
+      </c>
+      <c r="H48" s="143"/>
+      <c r="I48" s="143" t="s">
+        <v>76</v>
+      </c>
+      <c r="J48" s="143"/>
+      <c r="K48" s="142"/>
+      <c r="L48" s="141"/>
+      <c r="M48" s="140"/>
+      <c r="N48" s="140"/>
+      <c r="O48" s="140"/>
+      <c r="P48" s="140"/>
+    </row>
+    <row r="49" spans="1:16" ht="5.25" customHeight="1">
+      <c r="K49" s="136"/>
+    </row>
+    <row r="50" spans="1:16" ht="15.75">
+      <c r="A50" s="139" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="138"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="138"/>
+      <c r="E50" s="138"/>
+      <c r="F50" s="138"/>
+      <c r="G50" s="138"/>
+      <c r="H50" s="138"/>
+      <c r="I50" s="138"/>
+      <c r="J50" s="138"/>
+      <c r="K50" s="138"/>
+      <c r="L50" s="138"/>
+      <c r="M50" s="138"/>
+      <c r="N50" s="138"/>
+      <c r="O50" s="138"/>
+      <c r="P50" s="138"/>
+    </row>
+    <row r="51" spans="1:16" ht="5.25" customHeight="1"/>
+    <row r="52" spans="1:16">
+      <c r="A52" s="137"/>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" s="136"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="135" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="1">
+    <mergeCell ref="O2:O7"/>
+  </mergeCells>
+  <pageMargins left="0.62992125984252001" right="0.23622047244093999" top="0.35433070866142002" bottom="0.55118110236219997" header="0.11811023622047" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="89" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;K04-044M&amp;"Arial,Normal"&amp;8ETCUT RECHERCHES S.A.S.
+22 rue du Moulin de la Garde – 44477 CARQUEFOU Cedex  (Nantes) FRANCE – Tel. +33 240 252 507 – www.metcutfrance.com
+S.A.S. au capital de 206 250€ - VAT FR10388107443 000 11</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>